<commit_message>
pq finished and fixed reading time bug
</commit_message>
<xml_diff>
--- a/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_instructions_toy.xlsx
+++ b/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_instructions_toy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-experiment-implementation/experiment_implementation/data/participant_questionnaire_toy_x_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC2B905-3C3F-2F44-9CF9-2252A9C43CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCC5553-B302-D545-BB06-6C07DB17402A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>pq_instructions</t>
   </si>
@@ -175,9 +175,6 @@
     <t>pq_final_message</t>
   </si>
   <si>
-    <t>Thank you for filling out our questionnaire. Remember that all data will be anonymised and treated confidentially. If you have finished answering all the questions, please click 'Submit', otherwise click 'Previous' to go back and finish the questionnaire.</t>
-  </si>
-  <si>
     <t>Final message shown in the last screen.</t>
   </si>
   <si>
@@ -245,13 +242,22 @@
   </si>
   <si>
     <t>pq_answer_for_lang</t>
+  </si>
+  <si>
+    <t>pq_check_and_change_answers</t>
+  </si>
+  <si>
+    <t>Please check all your answers carefully. If you want to change an answer, tick the box next to it.</t>
+  </si>
+  <si>
+    <t>Thank you for filling out our questionnaire. Remember that all data will be anonymised and treated confidentially.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -384,6 +390,12 @@
       <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -728,8 +740,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1105,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:B30"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1332,94 +1345,102 @@
         <v>50</v>
       </c>
       <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
         <v>51</v>
-      </c>
-      <c r="C21" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
         <v>56</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>57</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
         <v>62</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
         <v>65</v>
-      </c>
-      <c r="B26" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
         <v>67</v>
-      </c>
-      <c r="B27" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
         <v>69</v>
-      </c>
-      <c r="B28" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
         <v>71</v>
-      </c>
-      <c r="B29" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B30" t="s">
-        <v>73</v>
+      <c r="B31" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add confirmation checkbox pq
</commit_message>
<xml_diff>
--- a/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_instructions_toy.xlsx
+++ b/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_instructions_toy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-experiment-implementation/experiment_implementation/data/participant_questionnaire_toy_x_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCC5553-B302-D545-BB06-6C07DB17402A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD406ED-752E-1A48-B775-742814E66EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t>pq_instructions</t>
   </si>
@@ -251,6 +251,18 @@
   </si>
   <si>
     <t>Thank you for filling out our questionnaire. Remember that all data will be anonymised and treated confidentially.</t>
+  </si>
+  <si>
+    <t>pq_confirmation</t>
+  </si>
+  <si>
+    <t>Please confirm that your answers are correct.</t>
+  </si>
+  <si>
+    <t>pq_confirm_answers</t>
+  </si>
+  <si>
+    <t>Please read your answers carefully one more time and check this box if they are correct. Then you can proceed.</t>
   </si>
 </sst>
 </file>
@@ -1118,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1443,6 +1455,22 @@
         <v>75</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>